<commit_message>
final rapor ilerlemesi yapıldı
</commit_message>
<xml_diff>
--- a/tidy_marriages.xlsx
+++ b/tidy_marriages.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yagmu\Desktop\emu660-spring2025-yyaslan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF0B270-609C-4423-8710-F5327A095887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69CEC58-0CD4-4329-808F-FC6BA6D728E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6254BE2-C0F6-44A1-A7BE-24E8D09363C5}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6254BE2-C0F6-44A1-A7BE-24E8D09363C5}"/>
   </bookViews>
   <sheets>
     <sheet name="37_t107" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'37_t107'!$A$1:$BI$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'37_t107'!$A$1:$BG$83</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'37_t107'!$A:$A,'37_t107'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -287,6 +287,9 @@
     </r>
   </si>
   <si>
+    <t>Year</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">
 </t>
@@ -298,7 +301,7 @@
         <family val="2"/>
         <charset val="162"/>
       </rPr>
-      <t>Year</t>
+      <t>Number_of_marriages</t>
     </r>
   </si>
   <si>
@@ -313,46 +316,11 @@
         <family val="2"/>
         <charset val="162"/>
       </rPr>
-      <t>Number of
-marriages</t>
+      <t>Number_of_marriages_between_first_cousins</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="162"/>
-      </rPr>
-      <t>Number of
-marriages
-between
-first cousins</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="162"/>
-      </rPr>
-      <t>Proportion
-of marriages
-between
-first cousins
-(%)</t>
-    </r>
+    <t>Proportion</t>
   </si>
 </sst>
 </file>
@@ -2179,7 +2147,7 @@
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="342" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2227,6 +2195,12 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1188">
@@ -3719,83 +3693,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF0D4AC-6E38-4CC3-8E3A-FB87E1AFDFDA}">
-  <dimension ref="A1:BI1395"/>
+  <dimension ref="A1:BG1395"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="2" width="14.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="1.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="1.5546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="1.5546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="1.5546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.88671875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="1.5546875" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="11.44140625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="1.5546875" style="3" customWidth="1"/>
-    <col min="27" max="27" width="9.88671875" style="3" customWidth="1"/>
-    <col min="28" max="28" width="11.88671875" style="3" customWidth="1"/>
-    <col min="29" max="29" width="11.44140625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="1.5546875" style="3" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" style="3" customWidth="1"/>
-    <col min="32" max="32" width="11.88671875" style="3" customWidth="1"/>
-    <col min="33" max="33" width="11.44140625" style="3" customWidth="1"/>
-    <col min="34" max="34" width="1.5546875" style="3" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" style="3" customWidth="1"/>
-    <col min="36" max="36" width="11.88671875" style="3" customWidth="1"/>
-    <col min="37" max="37" width="11.44140625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="1.5546875" style="3" customWidth="1"/>
-    <col min="39" max="39" width="9.88671875" style="3" customWidth="1"/>
-    <col min="40" max="40" width="11.88671875" style="3" customWidth="1"/>
-    <col min="41" max="41" width="11.44140625" style="3" customWidth="1"/>
-    <col min="42" max="42" width="1.5546875" style="3" customWidth="1"/>
-    <col min="43" max="43" width="9.88671875" style="3" customWidth="1"/>
-    <col min="44" max="44" width="11.88671875" style="3" customWidth="1"/>
-    <col min="45" max="45" width="11.44140625" style="3" customWidth="1"/>
-    <col min="46" max="46" width="1.5546875" style="3" customWidth="1"/>
-    <col min="47" max="47" width="9.88671875" style="3" customWidth="1"/>
-    <col min="48" max="48" width="11.88671875" style="3" customWidth="1"/>
-    <col min="49" max="49" width="11.44140625" style="3" customWidth="1"/>
-    <col min="50" max="50" width="1.5546875" style="3" customWidth="1"/>
-    <col min="51" max="51" width="9.88671875" style="3" customWidth="1"/>
-    <col min="52" max="52" width="11.88671875" style="3" customWidth="1"/>
-    <col min="53" max="53" width="11.44140625" style="3" customWidth="1"/>
-    <col min="54" max="54" width="1.5546875" style="3" customWidth="1"/>
-    <col min="55" max="55" width="9.88671875" style="3" customWidth="1"/>
-    <col min="56" max="56" width="11.88671875" style="3" customWidth="1"/>
-    <col min="57" max="57" width="11.44140625" style="3" customWidth="1"/>
-    <col min="58" max="58" width="1.5546875" style="3" customWidth="1"/>
-    <col min="59" max="59" width="9.88671875" style="3" customWidth="1"/>
-    <col min="60" max="60" width="11.88671875" style="3" customWidth="1"/>
-    <col min="61" max="61" width="11.44140625" style="3" customWidth="1"/>
-    <col min="62" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="2" width="14.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="1.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="1.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="1.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="1.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="3" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="1.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" style="3" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="1.5703125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="9.85546875" style="3" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" style="3" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="3" customWidth="1"/>
+    <col min="32" max="32" width="1.5703125" style="3" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" style="3" customWidth="1"/>
+    <col min="34" max="34" width="11.85546875" style="3" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" style="3" customWidth="1"/>
+    <col min="36" max="36" width="1.5703125" style="3" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" style="3" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" style="3" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" style="3" customWidth="1"/>
+    <col min="40" max="40" width="1.5703125" style="3" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" style="3" customWidth="1"/>
+    <col min="42" max="42" width="11.85546875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="11.42578125" style="3" customWidth="1"/>
+    <col min="44" max="44" width="1.5703125" style="3" customWidth="1"/>
+    <col min="45" max="45" width="9.85546875" style="3" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" style="3" customWidth="1"/>
+    <col min="47" max="47" width="11.42578125" style="3" customWidth="1"/>
+    <col min="48" max="48" width="1.5703125" style="3" customWidth="1"/>
+    <col min="49" max="49" width="9.85546875" style="3" customWidth="1"/>
+    <col min="50" max="50" width="11.85546875" style="3" customWidth="1"/>
+    <col min="51" max="51" width="11.42578125" style="3" customWidth="1"/>
+    <col min="52" max="52" width="1.5703125" style="3" customWidth="1"/>
+    <col min="53" max="53" width="9.85546875" style="3" customWidth="1"/>
+    <col min="54" max="54" width="11.85546875" style="3" customWidth="1"/>
+    <col min="55" max="55" width="11.42578125" style="3" customWidth="1"/>
+    <col min="56" max="56" width="1.5703125" style="3" customWidth="1"/>
+    <col min="57" max="57" width="9.85546875" style="3" customWidth="1"/>
+    <col min="58" max="58" width="11.85546875" style="3" customWidth="1"/>
+    <col min="59" max="59" width="11.42578125" style="3" customWidth="1"/>
+    <col min="60" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="98.25" customHeight="1">
+    <row r="1" spans="1:59" ht="98.25" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C1" s="16" t="s">
@@ -3804,67 +3776,65 @@
       <c r="D1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="19" t="s">
         <v>86</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="16"/>
-      <c r="N1" s="6"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="P1" s="6"/>
       <c r="Q1" s="16"/>
-      <c r="R1" s="6"/>
+      <c r="R1" s="16"/>
       <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
+      <c r="T1" s="6"/>
       <c r="U1" s="16"/>
-      <c r="V1" s="6"/>
+      <c r="V1" s="16"/>
       <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
+      <c r="X1" s="6"/>
       <c r="Y1" s="16"/>
-      <c r="Z1" s="6"/>
+      <c r="Z1" s="16"/>
       <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
+      <c r="AB1" s="6"/>
       <c r="AC1" s="16"/>
-      <c r="AD1" s="6"/>
+      <c r="AD1" s="16"/>
       <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
+      <c r="AF1" s="6"/>
       <c r="AG1" s="16"/>
-      <c r="AH1" s="6"/>
+      <c r="AH1" s="16"/>
       <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
+      <c r="AJ1" s="6"/>
       <c r="AK1" s="16"/>
-      <c r="AL1" s="6"/>
+      <c r="AL1" s="16"/>
       <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
+      <c r="AN1" s="6"/>
       <c r="AO1" s="16"/>
-      <c r="AP1" s="6"/>
+      <c r="AP1" s="16"/>
       <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
+      <c r="AR1" s="6"/>
       <c r="AS1" s="16"/>
-      <c r="AT1" s="6"/>
+      <c r="AT1" s="16"/>
       <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
+      <c r="AV1" s="6"/>
       <c r="AW1" s="16"/>
-      <c r="AX1" s="6"/>
+      <c r="AX1" s="16"/>
       <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
+      <c r="AZ1" s="6"/>
       <c r="BA1" s="16"/>
-      <c r="BB1" s="6"/>
+      <c r="BB1" s="16"/>
       <c r="BC1" s="16"/>
-      <c r="BD1" s="16"/>
+      <c r="BD1" s="6"/>
       <c r="BE1" s="16"/>
-      <c r="BF1" s="6"/>
+      <c r="BF1" s="16"/>
       <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-    </row>
-    <row r="2" spans="1:61" s="4" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:59" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>81</v>
       </c>
@@ -3882,7 +3852,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:61" ht="15" customHeight="1">
+    <row r="3" spans="1:59" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>80</v>
       </c>
@@ -3900,7 +3870,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:61" ht="15" customHeight="1">
+    <row r="4" spans="1:59" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
@@ -3918,7 +3888,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:61" ht="15" customHeight="1">
+    <row r="5" spans="1:59" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
@@ -3936,7 +3906,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:61" ht="15" customHeight="1">
+    <row r="6" spans="1:59" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -3954,7 +3924,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:61" ht="15" customHeight="1">
+    <row r="7" spans="1:59" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>76</v>
       </c>
@@ -3972,7 +3942,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:61" ht="15" customHeight="1">
+    <row r="8" spans="1:59" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>75</v>
       </c>
@@ -3990,7 +3960,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:61" ht="15" customHeight="1">
+    <row r="9" spans="1:59" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -4008,7 +3978,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:61" ht="15" customHeight="1">
+    <row r="10" spans="1:59" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>73</v>
       </c>
@@ -4026,7 +3996,7 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:61" ht="15" customHeight="1">
+    <row r="11" spans="1:59" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
@@ -4044,7 +4014,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:61" ht="15" customHeight="1">
+    <row r="12" spans="1:59" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
@@ -4062,7 +4032,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:61" ht="15" customHeight="1">
+    <row r="13" spans="1:59" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>70</v>
       </c>
@@ -4080,7 +4050,7 @@
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:61" ht="15" customHeight="1">
+    <row r="14" spans="1:59" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -4098,7 +4068,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:61" ht="15" customHeight="1">
+    <row r="15" spans="1:59" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
@@ -4116,7 +4086,7 @@
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:61" ht="15" customHeight="1">
+    <row r="16" spans="1:59" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
@@ -5340,7 +5310,7 @@
       </c>
       <c r="F83" s="11"/>
     </row>
-    <row r="84" spans="1:6" ht="12.9" customHeight="1">
+    <row r="84" spans="1:6" ht="12.95" customHeight="1">
       <c r="A84" s="12" t="s">
         <v>81</v>
       </c>
@@ -5358,7 +5328,7 @@
       </c>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="1:6" ht="12.9" customHeight="1">
+    <row r="85" spans="1:6" ht="12.95" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>80</v>
       </c>
@@ -6798,7 +6768,7 @@
       </c>
       <c r="F164" s="10"/>
     </row>
-    <row r="165" spans="1:6" ht="12" thickBot="1">
+    <row r="165" spans="1:6" ht="12.75" thickBot="1">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -6816,7 +6786,7 @@
       </c>
       <c r="F165" s="11"/>
     </row>
-    <row r="166" spans="1:6" ht="12">
+    <row r="166" spans="1:6">
       <c r="A166" s="12" t="s">
         <v>81</v>
       </c>
@@ -8274,7 +8244,7 @@
       </c>
       <c r="F246" s="10"/>
     </row>
-    <row r="247" spans="1:6" ht="12" thickBot="1">
+    <row r="247" spans="1:6" ht="12.75" thickBot="1">
       <c r="A247" s="1" t="s">
         <v>0</v>
       </c>
@@ -8292,7 +8262,7 @@
       </c>
       <c r="F247" s="11"/>
     </row>
-    <row r="248" spans="1:6" ht="12">
+    <row r="248" spans="1:6">
       <c r="A248" s="12" t="s">
         <v>81</v>
       </c>
@@ -9750,7 +9720,7 @@
       </c>
       <c r="F328" s="10"/>
     </row>
-    <row r="329" spans="1:6" ht="12" thickBot="1">
+    <row r="329" spans="1:6" ht="12.75" thickBot="1">
       <c r="A329" s="1" t="s">
         <v>0</v>
       </c>
@@ -9768,7 +9738,7 @@
       </c>
       <c r="F329" s="11"/>
     </row>
-    <row r="330" spans="1:6" ht="12">
+    <row r="330" spans="1:6">
       <c r="A330" s="12" t="s">
         <v>81</v>
       </c>
@@ -11226,7 +11196,7 @@
       </c>
       <c r="F410" s="10"/>
     </row>
-    <row r="411" spans="1:6" ht="12" thickBot="1">
+    <row r="411" spans="1:6" ht="12.75" thickBot="1">
       <c r="A411" s="1" t="s">
         <v>0</v>
       </c>
@@ -11244,7 +11214,7 @@
       </c>
       <c r="F411" s="11"/>
     </row>
-    <row r="412" spans="1:6" ht="12">
+    <row r="412" spans="1:6">
       <c r="A412" s="12" t="s">
         <v>81</v>
       </c>
@@ -12702,7 +12672,7 @@
       </c>
       <c r="F492" s="10"/>
     </row>
-    <row r="493" spans="1:6" ht="12" thickBot="1">
+    <row r="493" spans="1:6" ht="12.75" thickBot="1">
       <c r="A493" s="1" t="s">
         <v>0</v>
       </c>
@@ -12720,7 +12690,7 @@
       </c>
       <c r="F493" s="11"/>
     </row>
-    <row r="494" spans="1:6" ht="12">
+    <row r="494" spans="1:6">
       <c r="A494" s="12" t="s">
         <v>81</v>
       </c>
@@ -14178,7 +14148,7 @@
       </c>
       <c r="F574" s="10"/>
     </row>
-    <row r="575" spans="1:6" ht="12" thickBot="1">
+    <row r="575" spans="1:6" ht="12.75" thickBot="1">
       <c r="A575" s="1" t="s">
         <v>0</v>
       </c>
@@ -14196,7 +14166,7 @@
       </c>
       <c r="F575" s="11"/>
     </row>
-    <row r="576" spans="1:6" ht="12">
+    <row r="576" spans="1:6">
       <c r="A576" s="12" t="s">
         <v>81</v>
       </c>
@@ -15654,7 +15624,7 @@
       </c>
       <c r="F656" s="10"/>
     </row>
-    <row r="657" spans="1:6" ht="12" thickBot="1">
+    <row r="657" spans="1:6" ht="12.75" thickBot="1">
       <c r="A657" s="1" t="s">
         <v>0</v>
       </c>
@@ -15672,7 +15642,7 @@
       </c>
       <c r="F657" s="11"/>
     </row>
-    <row r="658" spans="1:6" ht="12">
+    <row r="658" spans="1:6">
       <c r="A658" s="12" t="s">
         <v>81</v>
       </c>
@@ -17130,7 +17100,7 @@
       </c>
       <c r="F738" s="10"/>
     </row>
-    <row r="739" spans="1:6" ht="12" thickBot="1">
+    <row r="739" spans="1:6" ht="12.75" thickBot="1">
       <c r="A739" s="1" t="s">
         <v>0</v>
       </c>
@@ -17148,7 +17118,7 @@
       </c>
       <c r="F739" s="11"/>
     </row>
-    <row r="740" spans="1:6" ht="12">
+    <row r="740" spans="1:6">
       <c r="A740" s="12" t="s">
         <v>81</v>
       </c>
@@ -18606,7 +18576,7 @@
       </c>
       <c r="F820" s="10"/>
     </row>
-    <row r="821" spans="1:6" ht="12" thickBot="1">
+    <row r="821" spans="1:6" ht="12.75" thickBot="1">
       <c r="A821" s="1" t="s">
         <v>0</v>
       </c>
@@ -18624,7 +18594,7 @@
       </c>
       <c r="F821" s="11"/>
     </row>
-    <row r="822" spans="1:6" ht="12">
+    <row r="822" spans="1:6">
       <c r="A822" s="12" t="s">
         <v>81</v>
       </c>
@@ -20082,7 +20052,7 @@
       </c>
       <c r="F902" s="10"/>
     </row>
-    <row r="903" spans="1:6" ht="12" thickBot="1">
+    <row r="903" spans="1:6" ht="12.75" thickBot="1">
       <c r="A903" s="1" t="s">
         <v>0</v>
       </c>
@@ -20100,7 +20070,7 @@
       </c>
       <c r="F903" s="11"/>
     </row>
-    <row r="904" spans="1:6" ht="12">
+    <row r="904" spans="1:6">
       <c r="A904" s="12" t="s">
         <v>81</v>
       </c>
@@ -21558,7 +21528,7 @@
       </c>
       <c r="F984" s="10"/>
     </row>
-    <row r="985" spans="1:6" ht="12" thickBot="1">
+    <row r="985" spans="1:6" ht="12.75" thickBot="1">
       <c r="A985" s="1" t="s">
         <v>0</v>
       </c>
@@ -21576,7 +21546,7 @@
       </c>
       <c r="F985" s="11"/>
     </row>
-    <row r="986" spans="1:6" ht="12">
+    <row r="986" spans="1:6">
       <c r="A986" s="12" t="s">
         <v>81</v>
       </c>
@@ -23034,7 +23004,7 @@
       </c>
       <c r="F1066" s="10"/>
     </row>
-    <row r="1067" spans="1:6" ht="12" thickBot="1">
+    <row r="1067" spans="1:6" ht="12.75" thickBot="1">
       <c r="A1067" s="1" t="s">
         <v>0</v>
       </c>
@@ -23052,7 +23022,7 @@
       </c>
       <c r="F1067" s="11"/>
     </row>
-    <row r="1068" spans="1:6" ht="12">
+    <row r="1068" spans="1:6">
       <c r="A1068" s="12" t="s">
         <v>81</v>
       </c>
@@ -24510,7 +24480,7 @@
       </c>
       <c r="F1148" s="10"/>
     </row>
-    <row r="1149" spans="1:6" ht="12" thickBot="1">
+    <row r="1149" spans="1:6" ht="12.75" thickBot="1">
       <c r="A1149" s="1" t="s">
         <v>0</v>
       </c>
@@ -24528,7 +24498,7 @@
       </c>
       <c r="F1149" s="11"/>
     </row>
-    <row r="1150" spans="1:6" ht="12">
+    <row r="1150" spans="1:6">
       <c r="A1150" s="12" t="s">
         <v>81</v>
       </c>
@@ -25905,7 +25875,7 @@
         <v>3.5928143712574849</v>
       </c>
     </row>
-    <row r="1231" spans="1:5" ht="12" thickBot="1">
+    <row r="1231" spans="1:5" ht="12.75" thickBot="1">
       <c r="A1231" s="1" t="s">
         <v>0</v>
       </c>
@@ -25922,7 +25892,7 @@
         <v>0.78515346181299073</v>
       </c>
     </row>
-    <row r="1232" spans="1:5" ht="12">
+    <row r="1232" spans="1:5">
       <c r="A1232" s="12"/>
       <c r="B1232" s="12"/>
     </row>
@@ -26246,11 +26216,11 @@
       <c r="A1312" s="2"/>
       <c r="B1312" s="2"/>
     </row>
-    <row r="1313" spans="1:2" ht="12" thickBot="1">
+    <row r="1313" spans="1:2" ht="12.75" thickBot="1">
       <c r="A1313" s="1"/>
       <c r="B1313" s="2"/>
     </row>
-    <row r="1314" spans="1:2" ht="12">
+    <row r="1314" spans="1:2">
       <c r="A1314" s="12"/>
       <c r="B1314" s="12"/>
     </row>
@@ -26574,7 +26544,7 @@
       <c r="A1394" s="2"/>
       <c r="B1394" s="2"/>
     </row>
-    <row r="1395" spans="1:2" ht="12" thickBot="1">
+    <row r="1395" spans="1:2" ht="12.75" thickBot="1">
       <c r="A1395" s="1"/>
       <c r="B1395" s="2"/>
     </row>

</xml_diff>